<commit_message>
Fix of the energy parameters
</commit_message>
<xml_diff>
--- a/ExperimentalData/ParametrosCineticos.xlsx
+++ b/ExperimentalData/ParametrosCineticos.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10511"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MARTA UCO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martadelarosanunez/Library/CloudStorage/OneDrive-Personal/Universidad/Code/GitHub/TFG_MartadelaRosa/ExperimentalData/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58696CD-31B7-934F-92EB-01DA74E0246B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>E</t>
   </si>
@@ -167,11 +168,14 @@
       <t>NR</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -503,16 +507,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -534,7 +538,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1.19</v>
       </c>
@@ -556,16 +560,16 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
-        <v>1.38</v>
+        <v>1.42</v>
       </c>
       <c r="B3" s="1">
         <v>141000000000000</v>
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1.68</v>
       </c>
@@ -574,34 +578,40 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
-        <v>1.78</v>
+        <v>1.85</v>
       </c>
       <c r="B5" s="1">
         <v>5780000000000000</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
-        <v>2.12</v>
+        <v>1.98</v>
       </c>
       <c r="B6" s="1">
         <v>8.71E+17</v>
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="B7" s="1">
         <v>1000000000000000</v>
       </c>
       <c r="D7" s="1"/>
     </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
(CODE): Meeting fixes. Correction of energy values. (LATEX): Chapter 3 and 4
</commit_message>
<xml_diff>
--- a/ExperimentalData/ParametrosCineticos.xlsx
+++ b/ExperimentalData/ParametrosCineticos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martadelarosanunez/Library/CloudStorage/OneDrive-Personal/Universidad/Code/GitHub/TFG_MartadelaRosa/ExperimentalData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58696CD-31B7-934F-92EB-01DA74E0246B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3DF44F-8931-714F-8BEC-803D1E1327CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6300" yWindow="-15660" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -511,7 +511,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -562,7 +562,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
-        <v>1.42</v>
+        <v>1.6</v>
       </c>
       <c r="B3" s="1">
         <v>141000000000000</v>
@@ -571,7 +571,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
-        <v>1.68</v>
+        <v>1.76</v>
       </c>
       <c r="B4" s="1">
         <v>9050000000000000</v>
@@ -580,7 +580,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
-        <v>1.85</v>
+        <v>1.87</v>
       </c>
       <c r="B5" s="1">
         <v>5780000000000000</v>

</xml_diff>